<commit_message>
Added Core BOM v025
Updated v024 to v025
</commit_message>
<xml_diff>
--- a/Bill of Materials/core-bom-v024.xlsx
+++ b/Bill of Materials/core-bom-v024.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -444,9 +444,6 @@
     <t>Song Ji</t>
   </si>
   <si>
-    <t>SJFC1332K12P20</t>
-  </si>
-  <si>
     <t>5032</t>
   </si>
   <si>
@@ -705,6 +702,9 @@
   </si>
   <si>
     <t>Non-inverting 3-state buffer</t>
+  </si>
+  <si>
+    <t>SJFC1332K07P20</t>
   </si>
 </sst>
 </file>
@@ -1938,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1964,12 +1964,12 @@
     </row>
     <row r="2" spans="2:10" ht="16" thickBot="1">
       <c r="B2" s="47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="48"/>
       <c r="D2" s="32">
         <f ca="1">TODAY()</f>
-        <v>41499</v>
+        <v>41508</v>
       </c>
     </row>
     <row r="3" spans="2:10">
@@ -1979,7 +1979,7 @@
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -1993,7 +1993,7 @@
         <v>93</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>86</v>
@@ -2016,10 +2016,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="46"/>
@@ -2036,22 +2036,22 @@
         <v>7</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H7" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="I7" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>151</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -2063,14 +2063,14 @@
         <v>7</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="39" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
@@ -2084,22 +2084,22 @@
         <v>7</v>
       </c>
       <c r="D9" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>125</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J9" s="5"/>
     </row>
@@ -2111,20 +2111,20 @@
         <v>7</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H10" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -2136,25 +2136,25 @@
         <v>54</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="2:10">
@@ -2165,25 +2165,25 @@
         <v>54</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="30">
@@ -2191,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>52</v>
@@ -2207,7 +2207,7 @@
         <v>94</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -2219,10 +2219,10 @@
         <v>49</v>
       </c>
       <c r="D14" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>22</v>
@@ -2250,7 +2250,7 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>39</v>
@@ -2259,10 +2259,10 @@
         <v>97</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="2:10">
@@ -2273,11 +2273,11 @@
         <v>1</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>11</v>
@@ -2286,7 +2286,7 @@
         <v>53</v>
       </c>
       <c r="I16" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J16" s="5"/>
     </row>
@@ -2314,7 +2314,7 @@
         <v>96</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="2:10">
@@ -2410,7 +2410,7 @@
         <v>42</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>68</v>
@@ -2450,7 +2450,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="20" t="s">
@@ -2463,7 +2463,7 @@
         <v>53</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -2475,7 +2475,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="20" t="s">
@@ -2485,10 +2485,10 @@
         <v>33</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -2500,7 +2500,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="20" t="s">
@@ -2513,7 +2513,7 @@
         <v>53</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J25" s="5"/>
     </row>
@@ -2525,7 +2525,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="20" t="s">
@@ -2538,7 +2538,7 @@
         <v>53</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J26" s="5"/>
     </row>
@@ -2550,7 +2550,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="20" t="s">
@@ -2563,7 +2563,7 @@
         <v>53</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J27" s="5"/>
     </row>
@@ -2575,7 +2575,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="20" t="s">
@@ -2588,7 +2588,7 @@
         <v>53</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J28" s="5"/>
     </row>
@@ -2610,7 +2610,7 @@
         <v>43</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>69</v>
@@ -2625,7 +2625,7 @@
         <v>82</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="22" t="s">
@@ -2638,7 +2638,7 @@
         <v>97</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>98</v>
+        <v>182</v>
       </c>
       <c r="J30" s="5"/>
     </row>
@@ -2647,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>78</v>
@@ -2675,7 +2675,7 @@
         <v>21</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="13" t="s">
@@ -2685,10 +2685,10 @@
         <v>31</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J32" s="5"/>
     </row>
@@ -2707,7 +2707,7 @@
         <v>22</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H33" s="15" t="s">
         <v>56</v>
@@ -2747,10 +2747,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="22" t="s">
@@ -2763,7 +2763,7 @@
         <v>60</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J35" s="5"/>
     </row>
@@ -2785,10 +2785,10 @@
         <v>3</v>
       </c>
       <c r="H36" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I36" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="J36" s="5"/>
     </row>
@@ -2805,13 +2805,13 @@
       <c r="E37" s="19"/>
       <c r="F37" s="5"/>
       <c r="G37" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H37" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="I37" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="I37" s="13" t="s">
-        <v>112</v>
       </c>
       <c r="J37" s="5"/>
     </row>
@@ -2820,26 +2820,26 @@
         <v>1</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E38" s="42"/>
       <c r="F38" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G38" s="41" t="s">
         <v>19</v>
       </c>
       <c r="H38" s="41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J38" s="40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="2:10">
@@ -2855,7 +2855,7 @@
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="28"/>
@@ -2877,7 +2877,7 @@
         <v>93</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>86</v>
@@ -2900,14 +2900,14 @@
         <v>1</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
@@ -2919,10 +2919,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="16" t="s">
@@ -2935,7 +2935,7 @@
     </row>
     <row r="45" spans="2:10">
       <c r="B45" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="2:10">
@@ -2949,7 +2949,7 @@
         <v>93</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>86</v>
@@ -2972,10 +2972,10 @@
         <v>1</v>
       </c>
       <c r="C47" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -2989,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D48" s="25"/>
       <c r="E48" s="25"/>

</xml_diff>